<commit_message>
Adicionei e retirei alguns ficheiros e mudei o nome de uns quantos para ficarem o mesmo nome.
</commit_message>
<xml_diff>
--- a/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 1/Sprint1/Sprint Backlog.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mafal\Desktop\college\third year (2022-2023)\first semester\classes\es\Projects\ganttproject\Project\Phase 1\Sprint1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD4FC0C-5857-4EA5-AAE3-75C5145C0C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="855" yWindow="-120" windowWidth="19755" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Folha1" sheetId="1" r:id="rId4"/>
+    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -229,47 +238,64 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font/>
-    <font>
-      <b/>
-      <sz val="14.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -277,7 +303,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -347,7 +373,13 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -361,27 +393,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -391,92 +430,98 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="12" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -666,390 +711,396 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="B2:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="10.88"/>
-    <col customWidth="1" min="3" max="3" width="12.63"/>
-    <col customWidth="1" min="4" max="4" width="5.75"/>
-    <col customWidth="1" min="5" max="5" width="15.0"/>
-    <col customWidth="1" min="6" max="6" width="17.63"/>
-    <col customWidth="1" min="7" max="7" width="16.25"/>
-    <col customWidth="1" min="8" max="9" width="15.0"/>
-    <col customWidth="1" min="10" max="10" width="34.25"/>
-    <col customWidth="1" min="11" max="11" width="27.0"/>
-    <col customWidth="1" min="12" max="12" width="25.88"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="9" width="25.7109375" customWidth="1"/>
+    <col min="10" max="10" width="39.7109375" customWidth="1"/>
+    <col min="11" max="11" width="29.28515625" customWidth="1"/>
+    <col min="12" max="12" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="26.25" customHeight="1">
+    <row r="2" spans="2:13" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="1"/>
       <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6" t="s">
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="B3" s="9" t="s">
+    <row r="3" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="10">
-        <v>44845.0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="7">
+        <v>44845</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
     </row>
-    <row r="4">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="10">
-        <v>44846.0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
+      <c r="C4" s="7">
+        <v>44846</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
     </row>
-    <row r="5">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="10">
-        <v>44847.0</v>
-      </c>
-      <c r="D5" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
+      <c r="C5" s="7">
+        <v>44847</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
-    <row r="6">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="10">
-        <v>44848.0</v>
-      </c>
-      <c r="D6" s="11">
-        <v>4.0</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+      <c r="C6" s="7">
+        <v>44848</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
     </row>
-    <row r="7">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="10">
-        <v>44849.0</v>
-      </c>
-      <c r="D7" s="11">
-        <v>5.0</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
+      <c r="C7" s="7">
+        <v>44849</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
     </row>
-    <row r="8">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10">
-        <v>44850.0</v>
-      </c>
-      <c r="D8" s="11">
-        <v>6.0</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="C8" s="7">
+        <v>44850</v>
+      </c>
+      <c r="D8" s="8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
     </row>
-    <row r="9">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="10">
-        <v>44851.0</v>
-      </c>
-      <c r="D9" s="11">
-        <v>7.0</v>
-      </c>
-      <c r="E9" s="18" t="s">
+      <c r="C9" s="7">
+        <v>44851</v>
+      </c>
+      <c r="D9" s="8">
+        <v>7</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="18" t="s">
+      <c r="F9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="16"/>
     </row>
-    <row r="10">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:13" ht="99.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10">
-        <v>44852.0</v>
-      </c>
-      <c r="D10" s="11">
-        <v>8.0</v>
-      </c>
-      <c r="E10" s="18" t="s">
+      <c r="C10" s="7">
+        <v>44852</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8</v>
+      </c>
+      <c r="E10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="I10" s="18" t="s">
+      <c r="H10" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="J10" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="18" t="s">
+      <c r="K10" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="M10" s="22"/>
+      <c r="M10" s="18"/>
     </row>
-    <row r="11">
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="2:13" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10">
-        <v>44853.0</v>
-      </c>
-      <c r="D11" s="11">
-        <v>9.0</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="C11" s="7">
+        <v>44853</v>
+      </c>
+      <c r="D11" s="8">
+        <v>9</v>
+      </c>
+      <c r="E11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18" t="s">
+      <c r="I11" s="15"/>
+      <c r="J11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="M11" s="23"/>
+      <c r="M11" s="19"/>
     </row>
-    <row r="12">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="2:13" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
-        <v>44854.0</v>
-      </c>
-      <c r="D12" s="11">
-        <v>10.0</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="C12" s="7">
+        <v>44854</v>
+      </c>
+      <c r="D12" s="8">
+        <v>10</v>
+      </c>
+      <c r="E12" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18" t="s">
+      <c r="I12" s="15"/>
+      <c r="J12" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="18" t="s">
+      <c r="K12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="10">
-        <v>44855.0</v>
-      </c>
-      <c r="D13" s="11">
-        <v>11.0</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="C13" s="7">
+        <v>44855</v>
+      </c>
+      <c r="D13" s="8">
+        <v>11</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18" t="s">
+      <c r="I13" s="15"/>
+      <c r="J13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="18" t="s">
+      <c r="K13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="23" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1058,8 +1109,7 @@
     <mergeCell ref="E2:I2"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="portrait" pageOrder="overThenDown"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="9" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd"/>
 </worksheet>
 </file>
</xml_diff>